<commit_message>
Fix ecdc-csv data for 2020-03-29.
</commit_message>
<xml_diff>
--- a/ecdc-csv/data/ecdc_csv_diff.xlsx
+++ b/ecdc-csv/data/ecdc_csv_diff.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="287">
   <si>
     <t>Date</t>
   </si>
@@ -874,6 +874,9 @@
   <si>
     <t>2020-03-28</t>
   </si>
+  <si>
+    <t>2020-03-29</t>
+  </si>
 </sst>
 </file>
 
@@ -1230,7 +1233,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:GO90"/>
+  <dimension ref="A1:GO91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -24242,6 +24245,596 @@
         <v>2</v>
       </c>
     </row>
+    <row r="91" spans="1:197">
+      <c r="A91" t="s">
+        <v>286</v>
+      </c>
+      <c r="B91">
+        <v>15</v>
+      </c>
+      <c r="C91">
+        <v>11</v>
+      </c>
+      <c r="D91">
+        <v>104</v>
+      </c>
+      <c r="E91">
+        <v>41</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>55</v>
+      </c>
+      <c r="J91">
+        <v>52</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>431</v>
+      </c>
+      <c r="M91">
+        <v>594</v>
+      </c>
+      <c r="N91">
+        <v>17</v>
+      </c>
+      <c r="O91">
+        <v>2</v>
+      </c>
+      <c r="P91">
+        <v>7</v>
+      </c>
+      <c r="Q91">
+        <v>0</v>
+      </c>
+      <c r="R91">
+        <v>2</v>
+      </c>
+      <c r="S91">
+        <v>0</v>
+      </c>
+      <c r="T91">
+        <v>1850</v>
+      </c>
+      <c r="U91">
+        <v>0</v>
+      </c>
+      <c r="V91">
+        <v>0</v>
+      </c>
+      <c r="W91">
+        <v>5</v>
+      </c>
+      <c r="X91">
+        <v>1</v>
+      </c>
+      <c r="Y91">
+        <v>7</v>
+      </c>
+      <c r="Z91">
+        <v>28</v>
+      </c>
+      <c r="AA91">
+        <v>487</v>
+      </c>
+      <c r="AB91">
+        <v>0</v>
+      </c>
+      <c r="AC91">
+        <v>5</v>
+      </c>
+      <c r="AD91">
+        <v>38</v>
+      </c>
+      <c r="AE91">
+        <v>34</v>
+      </c>
+      <c r="AF91">
+        <v>1</v>
+      </c>
+      <c r="AG91">
+        <v>11</v>
+      </c>
+      <c r="AH91">
+        <v>697</v>
+      </c>
+      <c r="AI91">
+        <v>1</v>
+      </c>
+      <c r="AK91">
+        <v>0</v>
+      </c>
+      <c r="AL91">
+        <v>1</v>
+      </c>
+      <c r="AM91">
+        <v>0</v>
+      </c>
+      <c r="AN91">
+        <v>299</v>
+      </c>
+      <c r="AO91">
+        <v>129</v>
+      </c>
+      <c r="AP91">
+        <v>69</v>
+      </c>
+      <c r="AQ91">
+        <v>15</v>
+      </c>
+      <c r="AR91">
+        <v>32</v>
+      </c>
+      <c r="AS91">
+        <v>39</v>
+      </c>
+      <c r="AT91">
+        <v>71</v>
+      </c>
+      <c r="AU91">
+        <v>39</v>
+      </c>
+      <c r="AV91">
+        <v>0</v>
+      </c>
+      <c r="AW91">
+        <v>17</v>
+      </c>
+      <c r="AX91">
+        <v>384</v>
+      </c>
+      <c r="AY91">
+        <v>0</v>
+      </c>
+      <c r="AZ91">
+        <v>155</v>
+      </c>
+      <c r="BA91">
+        <v>2</v>
+      </c>
+      <c r="BB91">
+        <v>0</v>
+      </c>
+      <c r="BC91">
+        <v>138</v>
+      </c>
+      <c r="BD91">
+        <v>208</v>
+      </c>
+      <c r="BE91">
+        <v>41</v>
+      </c>
+      <c r="BF91">
+        <v>6</v>
+      </c>
+      <c r="BG91">
+        <v>0</v>
+      </c>
+      <c r="BH91">
+        <v>0</v>
+      </c>
+      <c r="BI91">
+        <v>65</v>
+      </c>
+      <c r="BJ91">
+        <v>0</v>
+      </c>
+      <c r="BK91">
+        <v>0</v>
+      </c>
+      <c r="BL91">
+        <v>11</v>
+      </c>
+      <c r="BM91">
+        <v>0</v>
+      </c>
+      <c r="BN91">
+        <v>193</v>
+      </c>
+      <c r="BO91">
+        <v>4611</v>
+      </c>
+      <c r="BP91">
+        <v>4</v>
+      </c>
+      <c r="BQ91">
+        <v>0</v>
+      </c>
+      <c r="BR91">
+        <v>0</v>
+      </c>
+      <c r="BS91">
+        <v>4</v>
+      </c>
+      <c r="BT91">
+        <v>3965</v>
+      </c>
+      <c r="BU91">
+        <v>4</v>
+      </c>
+      <c r="BV91">
+        <v>1</v>
+      </c>
+      <c r="BW91">
+        <v>95</v>
+      </c>
+      <c r="BX91">
+        <v>1</v>
+      </c>
+      <c r="BY91">
+        <v>2</v>
+      </c>
+      <c r="BZ91">
+        <v>4</v>
+      </c>
+      <c r="CA91">
+        <v>2</v>
+      </c>
+      <c r="CB91">
+        <v>3</v>
+      </c>
+      <c r="CC91">
+        <v>3</v>
+      </c>
+      <c r="CD91">
+        <v>0</v>
+      </c>
+      <c r="CE91">
+        <v>3</v>
+      </c>
+      <c r="CF91">
+        <v>0</v>
+      </c>
+      <c r="CG91">
+        <v>1</v>
+      </c>
+      <c r="CH91">
+        <v>15</v>
+      </c>
+      <c r="CI91">
+        <v>65</v>
+      </c>
+      <c r="CJ91">
+        <v>73</v>
+      </c>
+      <c r="CK91">
+        <v>106</v>
+      </c>
+      <c r="CL91">
+        <v>109</v>
+      </c>
+      <c r="CM91">
+        <v>3076</v>
+      </c>
+      <c r="CN91">
+        <v>48</v>
+      </c>
+      <c r="CO91">
+        <v>294</v>
+      </c>
+      <c r="CP91">
+        <v>3</v>
+      </c>
+      <c r="CQ91">
+        <v>584</v>
+      </c>
+      <c r="CR91">
+        <v>5974</v>
+      </c>
+      <c r="CS91">
+        <v>6</v>
+      </c>
+      <c r="CT91">
+        <v>194</v>
+      </c>
+      <c r="CU91">
+        <v>9</v>
+      </c>
+      <c r="CV91">
+        <v>23</v>
+      </c>
+      <c r="CW91">
+        <v>36</v>
+      </c>
+      <c r="CX91">
+        <v>7</v>
+      </c>
+      <c r="CY91">
+        <v>0</v>
+      </c>
+      <c r="CZ91">
+        <v>10</v>
+      </c>
+      <c r="DA91">
+        <v>26</v>
+      </c>
+      <c r="DB91">
+        <v>0</v>
+      </c>
+      <c r="DC91">
+        <v>25</v>
+      </c>
+      <c r="DD91">
+        <v>21</v>
+      </c>
+      <c r="DE91">
+        <v>0</v>
+      </c>
+      <c r="DF91">
+        <v>0</v>
+      </c>
+      <c r="DG91">
+        <v>1</v>
+      </c>
+      <c r="DH91">
+        <v>36</v>
+      </c>
+      <c r="DI91">
+        <v>226</v>
+      </c>
+      <c r="DJ91">
+        <v>4</v>
+      </c>
+      <c r="DK91">
+        <v>159</v>
+      </c>
+      <c r="DL91">
+        <v>2</v>
+      </c>
+      <c r="DM91">
+        <v>5</v>
+      </c>
+      <c r="DN91">
+        <v>0</v>
+      </c>
+      <c r="DO91">
+        <v>2</v>
+      </c>
+      <c r="DP91">
+        <v>8</v>
+      </c>
+      <c r="DQ91">
+        <v>131</v>
+      </c>
+      <c r="DR91">
+        <v>32</v>
+      </c>
+      <c r="DS91">
+        <v>1</v>
+      </c>
+      <c r="DT91">
+        <v>1</v>
+      </c>
+      <c r="DU91">
+        <v>9</v>
+      </c>
+      <c r="DV91">
+        <v>0</v>
+      </c>
+      <c r="DW91">
+        <v>13</v>
+      </c>
+      <c r="DX91">
+        <v>1</v>
+      </c>
+      <c r="DY91">
+        <v>3</v>
+      </c>
+      <c r="DZ91">
+        <v>0</v>
+      </c>
+      <c r="EA91">
+        <v>2</v>
+      </c>
+      <c r="EB91">
+        <v>1159</v>
+      </c>
+      <c r="EC91">
+        <v>0</v>
+      </c>
+      <c r="ED91">
+        <v>60</v>
+      </c>
+      <c r="EE91">
+        <v>1</v>
+      </c>
+      <c r="EF91">
+        <v>0</v>
+      </c>
+      <c r="EG91">
+        <v>16</v>
+      </c>
+      <c r="EH91">
+        <v>22</v>
+      </c>
+      <c r="EI91">
+        <v>264</v>
+      </c>
+      <c r="EJ91">
+        <v>21</v>
+      </c>
+      <c r="EK91">
+        <v>211</v>
+      </c>
+      <c r="EL91">
+        <v>6</v>
+      </c>
+      <c r="EM91">
+        <v>115</v>
+      </c>
+      <c r="EN91">
+        <v>0</v>
+      </c>
+      <c r="EO91">
+        <v>3</v>
+      </c>
+      <c r="EP91">
+        <v>36</v>
+      </c>
+      <c r="EQ91">
+        <v>272</v>
+      </c>
+      <c r="ER91">
+        <v>249</v>
+      </c>
+      <c r="ES91">
+        <v>902</v>
+      </c>
+      <c r="ET91">
+        <v>36</v>
+      </c>
+      <c r="EU91">
+        <v>28</v>
+      </c>
+      <c r="EV91">
+        <v>160</v>
+      </c>
+      <c r="EW91">
+        <v>228</v>
+      </c>
+      <c r="EX91">
+        <v>6</v>
+      </c>
+      <c r="EY91">
+        <v>0</v>
+      </c>
+      <c r="EZ91">
+        <v>1</v>
+      </c>
+      <c r="FA91">
+        <v>0</v>
+      </c>
+      <c r="FB91">
+        <v>1</v>
+      </c>
+      <c r="FC91">
+        <v>99</v>
+      </c>
+      <c r="FD91">
+        <v>11</v>
+      </c>
+      <c r="FE91">
+        <v>202</v>
+      </c>
+      <c r="FF91">
+        <v>0</v>
+      </c>
+      <c r="FG91">
+        <v>71</v>
+      </c>
+      <c r="FH91">
+        <v>0</v>
+      </c>
+      <c r="FI91">
+        <v>0</v>
+      </c>
+      <c r="FJ91">
+        <v>59</v>
+      </c>
+      <c r="FK91">
+        <v>0</v>
+      </c>
+      <c r="FL91">
+        <v>17</v>
+      </c>
+      <c r="FM91">
+        <v>105</v>
+      </c>
+      <c r="FN91">
+        <v>8189</v>
+      </c>
+      <c r="FO91">
+        <v>9</v>
+      </c>
+      <c r="FP91">
+        <v>2</v>
+      </c>
+      <c r="FQ91">
+        <v>0</v>
+      </c>
+      <c r="FR91">
+        <v>401</v>
+      </c>
+      <c r="FS91">
+        <v>1048</v>
+      </c>
+      <c r="FT91">
+        <v>0</v>
+      </c>
+      <c r="FU91">
+        <v>16</v>
+      </c>
+      <c r="FV91">
+        <v>109</v>
+      </c>
+      <c r="FW91">
+        <v>0</v>
+      </c>
+      <c r="FX91">
+        <v>3</v>
+      </c>
+      <c r="FY91">
+        <v>8</v>
+      </c>
+      <c r="FZ91">
+        <v>0</v>
+      </c>
+      <c r="GA91">
+        <v>1704</v>
+      </c>
+      <c r="GB91">
+        <v>3</v>
+      </c>
+      <c r="GC91">
+        <v>16</v>
+      </c>
+      <c r="GD91">
+        <v>93</v>
+      </c>
+      <c r="GE91">
+        <v>63</v>
+      </c>
+      <c r="GF91">
+        <v>2546</v>
+      </c>
+      <c r="GG91">
+        <v>0</v>
+      </c>
+      <c r="GH91">
+        <v>3</v>
+      </c>
+      <c r="GI91">
+        <v>19979</v>
+      </c>
+      <c r="GJ91">
+        <v>66</v>
+      </c>
+      <c r="GK91">
+        <v>29</v>
+      </c>
+      <c r="GL91">
+        <v>0</v>
+      </c>
+      <c r="GM91">
+        <v>54</v>
+      </c>
+      <c r="GN91">
+        <v>12</v>
+      </c>
+      <c r="GO91">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24249,7 +24842,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:GO90"/>
+  <dimension ref="A1:GO91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -47261,6 +47854,596 @@
         <v>0</v>
       </c>
     </row>
+    <row r="91" spans="1:197">
+      <c r="A91" t="s">
+        <v>286</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>5</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>2</v>
+      </c>
+      <c r="J91">
+        <v>2</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>1</v>
+      </c>
+      <c r="M91">
+        <v>0</v>
+      </c>
+      <c r="N91">
+        <v>1</v>
+      </c>
+      <c r="O91">
+        <v>0</v>
+      </c>
+      <c r="P91">
+        <v>0</v>
+      </c>
+      <c r="Q91">
+        <v>0</v>
+      </c>
+      <c r="R91">
+        <v>0</v>
+      </c>
+      <c r="S91">
+        <v>0</v>
+      </c>
+      <c r="T91">
+        <v>64</v>
+      </c>
+      <c r="U91">
+        <v>0</v>
+      </c>
+      <c r="V91">
+        <v>0</v>
+      </c>
+      <c r="W91">
+        <v>0</v>
+      </c>
+      <c r="X91">
+        <v>0</v>
+      </c>
+      <c r="Y91">
+        <v>0</v>
+      </c>
+      <c r="Z91">
+        <v>2</v>
+      </c>
+      <c r="AA91">
+        <v>22</v>
+      </c>
+      <c r="AB91">
+        <v>0</v>
+      </c>
+      <c r="AC91">
+        <v>1</v>
+      </c>
+      <c r="AD91">
+        <v>4</v>
+      </c>
+      <c r="AE91">
+        <v>6</v>
+      </c>
+      <c r="AF91">
+        <v>0</v>
+      </c>
+      <c r="AG91">
+        <v>1</v>
+      </c>
+      <c r="AH91">
+        <v>7</v>
+      </c>
+      <c r="AI91">
+        <v>0</v>
+      </c>
+      <c r="AK91">
+        <v>0</v>
+      </c>
+      <c r="AL91">
+        <v>0</v>
+      </c>
+      <c r="AM91">
+        <v>0</v>
+      </c>
+      <c r="AN91">
+        <v>1</v>
+      </c>
+      <c r="AO91">
+        <v>5</v>
+      </c>
+      <c r="AP91">
+        <v>0</v>
+      </c>
+      <c r="AQ91">
+        <v>0</v>
+      </c>
+      <c r="AR91">
+        <v>0</v>
+      </c>
+      <c r="AS91">
+        <v>0</v>
+      </c>
+      <c r="AT91">
+        <v>2</v>
+      </c>
+      <c r="AU91">
+        <v>1</v>
+      </c>
+      <c r="AV91">
+        <v>0</v>
+      </c>
+      <c r="AW91">
+        <v>0</v>
+      </c>
+      <c r="AX91">
+        <v>2</v>
+      </c>
+      <c r="AY91">
+        <v>2</v>
+      </c>
+      <c r="AZ91">
+        <v>13</v>
+      </c>
+      <c r="BA91">
+        <v>0</v>
+      </c>
+      <c r="BB91">
+        <v>0</v>
+      </c>
+      <c r="BC91">
+        <v>8</v>
+      </c>
+      <c r="BD91">
+        <v>7</v>
+      </c>
+      <c r="BE91">
+        <v>6</v>
+      </c>
+      <c r="BF91">
+        <v>0</v>
+      </c>
+      <c r="BG91">
+        <v>0</v>
+      </c>
+      <c r="BH91">
+        <v>0</v>
+      </c>
+      <c r="BI91">
+        <v>0</v>
+      </c>
+      <c r="BJ91">
+        <v>0</v>
+      </c>
+      <c r="BK91">
+        <v>0</v>
+      </c>
+      <c r="BL91">
+        <v>0</v>
+      </c>
+      <c r="BM91">
+        <v>0</v>
+      </c>
+      <c r="BN91">
+        <v>2</v>
+      </c>
+      <c r="BO91">
+        <v>319</v>
+      </c>
+      <c r="BP91">
+        <v>0</v>
+      </c>
+      <c r="BQ91">
+        <v>0</v>
+      </c>
+      <c r="BR91">
+        <v>0</v>
+      </c>
+      <c r="BS91">
+        <v>0</v>
+      </c>
+      <c r="BT91">
+        <v>64</v>
+      </c>
+      <c r="BU91">
+        <v>2</v>
+      </c>
+      <c r="BV91">
+        <v>0</v>
+      </c>
+      <c r="BW91">
+        <v>4</v>
+      </c>
+      <c r="BX91">
+        <v>0</v>
+      </c>
+      <c r="BY91">
+        <v>0</v>
+      </c>
+      <c r="BZ91">
+        <v>0</v>
+      </c>
+      <c r="CA91">
+        <v>0</v>
+      </c>
+      <c r="CB91">
+        <v>0</v>
+      </c>
+      <c r="CC91">
+        <v>0</v>
+      </c>
+      <c r="CD91">
+        <v>0</v>
+      </c>
+      <c r="CE91">
+        <v>0</v>
+      </c>
+      <c r="CF91">
+        <v>0</v>
+      </c>
+      <c r="CG91">
+        <v>0</v>
+      </c>
+      <c r="CH91">
+        <v>1</v>
+      </c>
+      <c r="CI91">
+        <v>2</v>
+      </c>
+      <c r="CJ91">
+        <v>0</v>
+      </c>
+      <c r="CK91">
+        <v>6</v>
+      </c>
+      <c r="CL91">
+        <v>15</v>
+      </c>
+      <c r="CM91">
+        <v>139</v>
+      </c>
+      <c r="CN91">
+        <v>2</v>
+      </c>
+      <c r="CO91">
+        <v>14</v>
+      </c>
+      <c r="CP91">
+        <v>0</v>
+      </c>
+      <c r="CQ91">
+        <v>2</v>
+      </c>
+      <c r="CR91">
+        <v>887</v>
+      </c>
+      <c r="CS91">
+        <v>0</v>
+      </c>
+      <c r="CT91">
+        <v>3</v>
+      </c>
+      <c r="CU91">
+        <v>0</v>
+      </c>
+      <c r="CV91">
+        <v>1</v>
+      </c>
+      <c r="CW91">
+        <v>0</v>
+      </c>
+      <c r="CX91">
+        <v>0</v>
+      </c>
+      <c r="CY91">
+        <v>0</v>
+      </c>
+      <c r="CZ91">
+        <v>0</v>
+      </c>
+      <c r="DA91">
+        <v>0</v>
+      </c>
+      <c r="DB91">
+        <v>0</v>
+      </c>
+      <c r="DC91">
+        <v>0</v>
+      </c>
+      <c r="DD91">
+        <v>1</v>
+      </c>
+      <c r="DE91">
+        <v>0</v>
+      </c>
+      <c r="DF91">
+        <v>0</v>
+      </c>
+      <c r="DG91">
+        <v>0</v>
+      </c>
+      <c r="DH91">
+        <v>2</v>
+      </c>
+      <c r="DI91">
+        <v>3</v>
+      </c>
+      <c r="DJ91">
+        <v>0</v>
+      </c>
+      <c r="DK91">
+        <v>1</v>
+      </c>
+      <c r="DL91">
+        <v>0</v>
+      </c>
+      <c r="DM91">
+        <v>0</v>
+      </c>
+      <c r="DN91">
+        <v>0</v>
+      </c>
+      <c r="DO91">
+        <v>0</v>
+      </c>
+      <c r="DP91">
+        <v>0</v>
+      </c>
+      <c r="DQ91">
+        <v>4</v>
+      </c>
+      <c r="DR91">
+        <v>0</v>
+      </c>
+      <c r="DS91">
+        <v>0</v>
+      </c>
+      <c r="DT91">
+        <v>0</v>
+      </c>
+      <c r="DU91">
+        <v>0</v>
+      </c>
+      <c r="DV91">
+        <v>0</v>
+      </c>
+      <c r="DW91">
+        <v>0</v>
+      </c>
+      <c r="DX91">
+        <v>0</v>
+      </c>
+      <c r="DY91">
+        <v>0</v>
+      </c>
+      <c r="DZ91">
+        <v>0</v>
+      </c>
+      <c r="EA91">
+        <v>0</v>
+      </c>
+      <c r="EB91">
+        <v>93</v>
+      </c>
+      <c r="EC91">
+        <v>0</v>
+      </c>
+      <c r="ED91">
+        <v>1</v>
+      </c>
+      <c r="EE91">
+        <v>0</v>
+      </c>
+      <c r="EF91">
+        <v>0</v>
+      </c>
+      <c r="EG91">
+        <v>0</v>
+      </c>
+      <c r="EH91">
+        <v>1</v>
+      </c>
+      <c r="EI91">
+        <v>4</v>
+      </c>
+      <c r="EJ91">
+        <v>0</v>
+      </c>
+      <c r="EK91">
+        <v>2</v>
+      </c>
+      <c r="EL91">
+        <v>0</v>
+      </c>
+      <c r="EM91">
+        <v>3</v>
+      </c>
+      <c r="EN91">
+        <v>0</v>
+      </c>
+      <c r="EO91">
+        <v>0</v>
+      </c>
+      <c r="EP91">
+        <v>5</v>
+      </c>
+      <c r="EQ91">
+        <v>14</v>
+      </c>
+      <c r="ER91">
+        <v>2</v>
+      </c>
+      <c r="ES91">
+        <v>24</v>
+      </c>
+      <c r="ET91">
+        <v>1</v>
+      </c>
+      <c r="EU91">
+        <v>1</v>
+      </c>
+      <c r="EV91">
+        <v>5</v>
+      </c>
+      <c r="EW91">
+        <v>1</v>
+      </c>
+      <c r="EX91">
+        <v>0</v>
+      </c>
+      <c r="EY91">
+        <v>0</v>
+      </c>
+      <c r="EZ91">
+        <v>0</v>
+      </c>
+      <c r="FA91">
+        <v>0</v>
+      </c>
+      <c r="FB91">
+        <v>1</v>
+      </c>
+      <c r="FC91">
+        <v>1</v>
+      </c>
+      <c r="FD91">
+        <v>0</v>
+      </c>
+      <c r="FE91">
+        <v>4</v>
+      </c>
+      <c r="FF91">
+        <v>0</v>
+      </c>
+      <c r="FG91">
+        <v>1</v>
+      </c>
+      <c r="FH91">
+        <v>0</v>
+      </c>
+      <c r="FI91">
+        <v>0</v>
+      </c>
+      <c r="FJ91">
+        <v>0</v>
+      </c>
+      <c r="FK91">
+        <v>0</v>
+      </c>
+      <c r="FL91">
+        <v>0</v>
+      </c>
+      <c r="FM91">
+        <v>8</v>
+      </c>
+      <c r="FN91">
+        <v>832</v>
+      </c>
+      <c r="FO91">
+        <v>1</v>
+      </c>
+      <c r="FP91">
+        <v>0</v>
+      </c>
+      <c r="FQ91">
+        <v>0</v>
+      </c>
+      <c r="FR91">
+        <v>10</v>
+      </c>
+      <c r="FS91">
+        <v>38</v>
+      </c>
+      <c r="FT91">
+        <v>0</v>
+      </c>
+      <c r="FU91">
+        <v>0</v>
+      </c>
+      <c r="FV91">
+        <v>1</v>
+      </c>
+      <c r="FW91">
+        <v>0</v>
+      </c>
+      <c r="FX91">
+        <v>0</v>
+      </c>
+      <c r="FY91">
+        <v>0</v>
+      </c>
+      <c r="FZ91">
+        <v>0</v>
+      </c>
+      <c r="GA91">
+        <v>16</v>
+      </c>
+      <c r="GB91">
+        <v>0</v>
+      </c>
+      <c r="GC91">
+        <v>0</v>
+      </c>
+      <c r="GD91">
+        <v>3</v>
+      </c>
+      <c r="GE91">
+        <v>0</v>
+      </c>
+      <c r="GF91">
+        <v>260</v>
+      </c>
+      <c r="GG91">
+        <v>1</v>
+      </c>
+      <c r="GH91">
+        <v>0</v>
+      </c>
+      <c r="GI91">
+        <v>484</v>
+      </c>
+      <c r="GJ91">
+        <v>0</v>
+      </c>
+      <c r="GK91">
+        <v>1</v>
+      </c>
+      <c r="GL91">
+        <v>0</v>
+      </c>
+      <c r="GM91">
+        <v>0</v>
+      </c>
+      <c r="GN91">
+        <v>0</v>
+      </c>
+      <c r="GO91">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>